<commit_message>
Dati emergenza pronti - visore aggiornato
</commit_message>
<xml_diff>
--- a/aggregated_medici_by_municipality.xlsx
+++ b/aggregated_medici_by_municipality.xlsx
@@ -6681,16 +6681,16 @@
         <v>1182</v>
       </c>
       <c r="C293" t="n">
-        <v>396.3190282007897</v>
+        <v>0.6135095882684714</v>
       </c>
       <c r="D293" t="n">
-        <v>253.251471141192</v>
+        <v>1.806749388982891</v>
       </c>
       <c r="E293" t="n">
-        <v>1.338014638417335</v>
+        <v>1.731142016287386</v>
       </c>
       <c r="F293" t="n">
-        <v>1.074121395600493</v>
+        <v>2.44697199772943</v>
       </c>
     </row>
     <row r="294">

</xml_diff>